<commit_message>
Atualização automática de VERANOPOLIS.xlsx
</commit_message>
<xml_diff>
--- a/VERANOPOLIS.xlsx
+++ b/VERANOPOLIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7F155EF-D783-4B25-9C9C-A65A71085944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71AEB377-4E33-4027-B79D-D92A28CAC06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{48AEE859-B3F4-41CA-9787-B511023A6C03}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{FAA6D50E-AEBF-4DA0-BC1B-030370B13487}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1240,10 +1240,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83374734-4D02-4A17-8DD7-E0713D5127C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC14FD7A-68A2-4396-8706-73C1A6697B9A}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,7 +1281,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9540D67-935F-4A2F-AFBA-FE72EA245238}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4792F8B-5526-4B24-93A1-C462C154223D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1344,7 +1344,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0D9C21C-1A1C-4394-BFB2-D8BEB1610872}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83D15AF5-B189-44E3-84B0-7B11B01B0A30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1363,7 +1363,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D437A6B-31F4-6DF4-C892-0CD1AA41E3AD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D1991C-F42F-30A7-04CC-92DF52886F01}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1412,7 +1412,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D7E2FBD-97DD-8332-7790-0B52F24E9DE7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A442C1FF-5599-D102-8260-21FAEC064CFD}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1431,7 +1431,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4B1318-EEA8-4BEB-D319-64696C214736}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A30CED-8E83-11D8-D066-42F02C40EC9F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1462,7 +1462,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88438BE4-87F4-6776-5FD2-F8B3D44498D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48BCBAEB-BFFA-0C03-1C8D-598C14530C9E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1493,7 +1493,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{672CD677-6D62-89E1-95B2-35F5803FB49A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30EE97BC-46C2-B0CC-5DBB-4CEFB0B003E8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1536,7 +1536,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C702A4E8-70A1-4A01-9614-6D65A206106B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F98202E-6B06-4B7E-B456-449EB2403832}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1574,7 +1574,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{851F93E3-A6F7-40A9-A810-794812B7A6C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CBE5ACE-91A0-437F-87E3-BD87E233251C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1617,7 +1617,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B29C7F9E-A263-4E69-B09B-AB0F043407C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0428CCC0-0DC2-4C20-9E00-8257C22D85A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1930,7 +1930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C7DD88-B8EC-4DBC-BF54-27366AA59E4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AAC345-7F19-4C2C-A112-FD84C7E069DF}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>